<commit_message>
Added works with chords
</commit_message>
<xml_diff>
--- a/Docs/WhatINeed.xlsx
+++ b/Docs/WhatINeed.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6C6AEE-7D33-4FAA-931D-31F73DA63242}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8A9B52-DD9A-4AE3-B541-FC750AF152D2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Что нужно</t>
   </si>
@@ -149,6 +149,12 @@
   </si>
   <si>
     <t>И так уже 2-а теста через свагер и фронт, сделаю потом когда будет что тестировать</t>
+  </si>
+  <si>
+    <t>Сделать isBlocked так что бы он был BlockContent</t>
+  </si>
+  <si>
+    <t>Сделать так что бы у блокировки было время</t>
   </si>
 </sst>
 </file>
@@ -578,7 +584,7 @@
   <dimension ref="A1:G4002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -848,12 +854,20 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
+      <c r="C20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="2"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="12">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
+      <c r="C21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="2"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="12">

</xml_diff>